<commit_message>
Multiple window handling code added
</commit_message>
<xml_diff>
--- a/target/test-classes/testData.xlsx
+++ b/target/test-classes/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jomjose/Documents/SeleniumProjects/internetherokuapp/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B30946-9C7E-6648-BC16-B3A75321020F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C845D3-FBEF-B143-953F-153B21002E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{9067BCB2-4237-DD4B-926D-C40B9C244DA0}"/>
   </bookViews>
@@ -44,10 +44,10 @@
     <t>Password</t>
   </si>
   <si>
-    <t> tomsmith</t>
+    <t>SuperSecretPassword!</t>
   </si>
   <si>
-    <t>SuperSecretPassword!</t>
+    <t>tomsmith</t>
   </si>
 </sst>
 </file>
@@ -402,10 +402,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -417,10 +420,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>